<commit_message>
Final staging before handing over to desktop
</commit_message>
<xml_diff>
--- a/debug.xlsx
+++ b/debug.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\UMAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Builtin</t>
   </si>
@@ -55,6 +54,9 @@
   </si>
   <si>
     <t>Calculated_Mises</t>
+  </si>
+  <si>
+    <t>SED</t>
   </si>
 </sst>
 </file>
@@ -126,7 +128,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -586,11 +587,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133854912"/>
-        <c:axId val="133855472"/>
+        <c:axId val="233387408"/>
+        <c:axId val="233387968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133854912"/>
+        <c:axId val="233387408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,12 +648,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133855472"/>
+        <c:crossAx val="233387968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133855472"/>
+        <c:axId val="233387968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,7 +710,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133854912"/>
+        <c:crossAx val="233387408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1614,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AC110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G30" workbookViewId="0">
-      <selection activeCell="U45" sqref="U45"/>
+    <sheetView tabSelected="1" topLeftCell="G51" workbookViewId="0">
+      <selection activeCell="S68" sqref="S68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2958,7 +2959,7 @@
         <v>3.9241099999999998E-3</v>
       </c>
       <c r="N30">
-        <f t="shared" ref="N30:N71" si="1">SQRT(0.5*((H30-I30)^2+(I30-J30)^2+(J30-H30)^2+6*(K30^2+L30^2+M30^2)))</f>
+        <f t="shared" ref="N30:N49" si="1">SQRT(0.5*((H30-I30)^2+(I30-J30)^2+(J30-H30)^2+6*(K30^2+L30^2+M30^2)))</f>
         <v>648.73264431239625</v>
       </c>
       <c r="P30">
@@ -4339,6 +4340,9 @@
       <c r="G50" t="s">
         <v>2</v>
       </c>
+      <c r="S50" t="s">
+        <v>10</v>
+      </c>
       <c r="X50">
         <v>0.40169100000000002</v>
       </c>
@@ -4369,6 +4373,12 @@
         <v>0</v>
       </c>
       <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>0</v>
+      </c>
+      <c r="T51">
         <v>0</v>
       </c>
       <c r="X51">
@@ -4403,6 +4413,12 @@
       <c r="Q52">
         <v>647.44500000000005</v>
       </c>
+      <c r="S52">
+        <v>0.05</v>
+      </c>
+      <c r="T52">
+        <v>0.62120600000000004</v>
+      </c>
       <c r="X52">
         <v>0.42169099999999998</v>
       </c>
@@ -4435,6 +4451,12 @@
       <c r="Q53">
         <v>2527.2199999999998</v>
       </c>
+      <c r="S53">
+        <v>0.1</v>
+      </c>
+      <c r="T53">
+        <v>2.77684</v>
+      </c>
       <c r="X53">
         <v>0.43169099999999999</v>
       </c>
@@ -4461,6 +4483,12 @@
       <c r="Q54">
         <v>5668.13</v>
       </c>
+      <c r="S54">
+        <v>0.15</v>
+      </c>
+      <c r="T54">
+        <v>7.3437099999999997</v>
+      </c>
       <c r="X54">
         <v>0.441691</v>
       </c>
@@ -4487,6 +4515,12 @@
       <c r="Q55">
         <v>10093</v>
       </c>
+      <c r="S55">
+        <v>0.2</v>
+      </c>
+      <c r="T55">
+        <v>15.789</v>
+      </c>
       <c r="X55">
         <v>0.45169100000000001</v>
       </c>
@@ -4513,6 +4547,12 @@
       <c r="Q56">
         <v>15854.2</v>
       </c>
+      <c r="S56">
+        <v>0.25</v>
+      </c>
+      <c r="T56">
+        <v>30.189800000000002</v>
+      </c>
       <c r="X56">
         <v>0.46169100000000002</v>
       </c>
@@ -4539,6 +4579,12 @@
       <c r="Q57">
         <v>23055.3</v>
       </c>
+      <c r="S57">
+        <v>0.3</v>
+      </c>
+      <c r="T57">
+        <v>53.283700000000003</v>
+      </c>
       <c r="X57">
         <v>0.47169100000000003</v>
       </c>
@@ -4565,6 +4611,12 @@
       <c r="Q58">
         <v>31881.3</v>
       </c>
+      <c r="S58">
+        <v>0.35</v>
+      </c>
+      <c r="T58">
+        <v>88.5732</v>
+      </c>
       <c r="X58">
         <v>0.48169099999999998</v>
       </c>
@@ -4591,6 +4643,12 @@
       <c r="Q59">
         <v>42641.2</v>
       </c>
+      <c r="S59">
+        <v>0.4</v>
+      </c>
+      <c r="T59">
+        <v>140.52000000000001</v>
+      </c>
       <c r="X59">
         <v>0.49169099999999999</v>
       </c>
@@ -4617,6 +4675,12 @@
       <c r="Q60">
         <v>55829.5</v>
       </c>
+      <c r="S60">
+        <v>0.45</v>
+      </c>
+      <c r="T60">
+        <v>214.88200000000001</v>
+      </c>
       <c r="X60">
         <v>0.501691</v>
       </c>
@@ -4643,6 +4707,12 @@
       <c r="Q61">
         <v>72218.8</v>
       </c>
+      <c r="S61">
+        <v>0.5</v>
+      </c>
+      <c r="T61">
+        <v>319.26600000000002</v>
+      </c>
       <c r="X61">
         <v>0.51169100000000001</v>
       </c>
@@ -4669,6 +4739,12 @@
       <c r="Q62">
         <v>93005.6</v>
       </c>
+      <c r="S62">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T62">
+        <v>464.04199999999997</v>
+      </c>
       <c r="X62">
         <v>0.52169100000000002</v>
       </c>
@@ -4695,6 +4771,12 @@
       <c r="Q63">
         <v>120049</v>
       </c>
+      <c r="S63">
+        <v>0.6</v>
+      </c>
+      <c r="T63">
+        <v>663.82100000000003</v>
+      </c>
       <c r="X63">
         <v>0.53169100000000002</v>
       </c>
@@ -4721,6 +4803,12 @@
       <c r="Q64">
         <v>156276</v>
       </c>
+      <c r="S64">
+        <v>0.65</v>
+      </c>
+      <c r="T64">
+        <v>939.91700000000003</v>
+      </c>
       <c r="X64">
         <v>0.54169100000000003</v>
       </c>
@@ -4747,6 +4835,12 @@
       <c r="Q65">
         <v>206383</v>
       </c>
+      <c r="S65">
+        <v>0.7</v>
+      </c>
+      <c r="T65">
+        <v>1324.48</v>
+      </c>
       <c r="X65">
         <v>0.55169100000000004</v>
       </c>
@@ -4773,6 +4867,12 @@
       <c r="Q66">
         <v>278115</v>
       </c>
+      <c r="S66">
+        <v>0.75</v>
+      </c>
+      <c r="T66">
+        <v>1867.71</v>
+      </c>
       <c r="X66">
         <v>0.56169100000000005</v>
       </c>
@@ -4799,6 +4899,12 @@
       <c r="Q67">
         <v>384642</v>
       </c>
+      <c r="S67">
+        <v>0.8</v>
+      </c>
+      <c r="T67">
+        <v>2650.73</v>
+      </c>
       <c r="X67">
         <v>0.57169099999999995</v>
       </c>
@@ -4825,6 +4931,12 @@
       <c r="Q68">
         <v>549183</v>
       </c>
+      <c r="S68">
+        <v>0.85</v>
+      </c>
+      <c r="T68">
+        <v>3809.57</v>
+      </c>
       <c r="X68">
         <v>0.58169099999999996</v>
       </c>
@@ -4851,6 +4963,12 @@
       <c r="Q69">
         <v>814335</v>
       </c>
+      <c r="S69">
+        <v>0.9</v>
+      </c>
+      <c r="T69">
+        <v>5581.48</v>
+      </c>
       <c r="X69">
         <v>0.59169099999999997</v>
       </c>
@@ -4877,6 +4995,12 @@
       <c r="Q70" s="1">
         <v>1261770</v>
       </c>
+      <c r="S70">
+        <v>0.95</v>
+      </c>
+      <c r="T70">
+        <v>8398.3700000000008</v>
+      </c>
       <c r="X70">
         <v>0.60169099999999998</v>
       </c>
@@ -4902,6 +5026,12 @@
       </c>
       <c r="Q71" s="1">
         <v>2055880</v>
+      </c>
+      <c r="S71">
+        <v>1</v>
+      </c>
+      <c r="T71">
+        <v>13084.4</v>
       </c>
       <c r="X71">
         <v>0.61169099999999998</v>

</xml_diff>